<commit_message>
Adding bat & icon
</commit_message>
<xml_diff>
--- a/data/daily_runoff/12256_Rosegbach_example_river_runoff.xlsx
+++ b/data/daily_runoff/12256_Rosegbach_example_river_runoff.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10114"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0639FD07-29BE-E644-A480-08CCBE4382B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5779F83D-27DA-094F-A786-60A6E695D738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14260" yWindow="760" windowWidth="15580" windowHeight="13360" tabRatio="841" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15420" yWindow="1640" windowWidth="14820" windowHeight="13360" tabRatio="841" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2000" sheetId="9" r:id="rId1"/>
@@ -38183,8 +38183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B366"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="B153" sqref="B153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -38660,508 +38660,790 @@
       <c r="A59" s="5">
         <v>37679</v>
       </c>
+      <c r="B59">
+        <v>0.08</v>
+      </c>
     </row>
     <row r="60" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="5">
         <v>37680</v>
       </c>
+      <c r="B60">
+        <v>0.09</v>
+      </c>
     </row>
     <row r="61" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="5">
         <v>37681</v>
       </c>
+      <c r="B61">
+        <v>0.09</v>
+      </c>
     </row>
     <row r="62" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="5">
         <v>37682</v>
       </c>
+      <c r="B62">
+        <v>0.09</v>
+      </c>
     </row>
     <row r="63" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="5">
         <v>37683</v>
       </c>
+      <c r="B63">
+        <v>0.09</v>
+      </c>
     </row>
     <row r="64" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="5">
         <v>37684</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B64">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="5">
         <v>37685</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B65">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="5">
         <v>37686</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B66">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="5">
         <v>37687</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B67">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="5">
         <v>37688</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B68">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="5">
         <v>37689</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B69">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="5">
         <v>37690</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B70">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="5">
         <v>37691</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B71">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="5">
         <v>37692</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B72">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="5">
         <v>37693</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B73">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="5">
         <v>37694</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B74">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="5">
         <v>37695</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B75">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="5">
         <v>37696</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B76">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" s="5">
         <v>37697</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B77">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A78" s="5">
         <v>37698</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B78">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="5">
         <v>37699</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B79">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="5">
         <v>37700</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B80">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A81" s="5">
         <v>37701</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B81">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A82" s="5">
         <v>37702</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B82">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A83" s="5">
         <v>37703</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B83">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" s="5">
         <v>37704</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B84">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" s="5">
         <v>37705</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B85">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A86" s="5">
         <v>37706</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B86">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="5">
         <v>37707</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B87">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A88" s="5">
         <v>37708</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B88">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A89" s="5">
         <v>37709</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B89">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A90" s="5">
         <v>37710</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B90">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="5">
         <v>37711</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B91">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A92" s="5">
         <v>37712</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B92">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A93" s="5">
         <v>37713</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B93">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A94" s="5">
         <v>37714</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B94">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A95" s="5">
         <v>37715</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B95">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A96" s="5">
         <v>37716</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B96">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A97" s="5">
         <v>37717</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B97">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A98" s="5">
         <v>37718</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B98">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A99" s="5">
         <v>37719</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B99">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A100" s="5">
         <v>37720</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B100">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A101" s="5">
         <v>37721</v>
       </c>
-    </row>
-    <row r="102" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B101">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A102" s="5">
         <v>37722</v>
       </c>
-    </row>
-    <row r="103" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B102">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A103" s="5">
         <v>37723</v>
       </c>
-    </row>
-    <row r="104" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B103">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A104" s="5">
         <v>37724</v>
       </c>
-    </row>
-    <row r="105" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B104">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A105" s="5">
         <v>37725</v>
       </c>
-    </row>
-    <row r="106" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B105">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A106" s="5">
         <v>37726</v>
       </c>
-    </row>
-    <row r="107" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B106">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A107" s="5">
         <v>37727</v>
       </c>
-    </row>
-    <row r="108" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B107">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A108" s="5">
         <v>37728</v>
       </c>
-    </row>
-    <row r="109" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B108">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A109" s="5">
         <v>37729</v>
       </c>
-    </row>
-    <row r="110" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B109">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A110" s="5">
         <v>37730</v>
       </c>
-    </row>
-    <row r="111" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B110">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A111" s="5">
         <v>37731</v>
       </c>
-    </row>
-    <row r="112" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B111">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A112" s="5">
         <v>37732</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B112">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A113" s="5">
         <v>37733</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B113">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A114" s="5">
         <v>37734</v>
       </c>
-    </row>
-    <row r="115" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B114">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A115" s="5">
         <v>37735</v>
       </c>
-    </row>
-    <row r="116" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B115">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A116" s="5">
         <v>37736</v>
       </c>
-    </row>
-    <row r="117" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B116">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A117" s="5">
         <v>37737</v>
       </c>
-    </row>
-    <row r="118" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B117">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A118" s="5">
         <v>37738</v>
       </c>
-    </row>
-    <row r="119" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B118">
+        <v>1.1399999999999999</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A119" s="5">
         <v>37739</v>
       </c>
-    </row>
-    <row r="120" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B119">
+        <v>1.18</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A120" s="5">
         <v>37740</v>
       </c>
-    </row>
-    <row r="121" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B120">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A121" s="5">
         <v>37741</v>
       </c>
-    </row>
-    <row r="122" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B121">
+        <v>1.66</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A122" s="5">
         <v>37742</v>
       </c>
-    </row>
-    <row r="123" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B122">
+        <v>3.47</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A123" s="5">
         <v>37743</v>
       </c>
-    </row>
-    <row r="124" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B123">
+        <v>2.66</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A124" s="5">
         <v>37744</v>
       </c>
-    </row>
-    <row r="125" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B124">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A125" s="5">
         <v>37745</v>
       </c>
-    </row>
-    <row r="126" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B125">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A126" s="5">
         <v>37746</v>
       </c>
-    </row>
-    <row r="127" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B126">
+        <v>2.2400000000000002</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A127" s="5">
         <v>37747</v>
       </c>
-    </row>
-    <row r="128" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B127">
+        <v>3.05</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A128" s="5">
         <v>37748</v>
       </c>
-    </row>
-    <row r="129" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B128">
+        <v>3.77</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A129" s="5">
         <v>37749</v>
       </c>
-    </row>
-    <row r="130" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B129">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A130" s="5">
         <v>37750</v>
       </c>
-    </row>
-    <row r="131" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B130">
+        <v>5.26</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A131" s="5">
         <v>37751</v>
       </c>
-    </row>
-    <row r="132" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B131">
+        <v>4.32</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A132" s="5">
         <v>37752</v>
       </c>
-    </row>
-    <row r="133" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B132">
+        <v>3.93</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A133" s="5">
         <v>37753</v>
       </c>
-    </row>
-    <row r="134" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B133">
+        <v>3.95</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A134" s="5">
         <v>37754</v>
       </c>
-    </row>
-    <row r="135" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B134">
+        <v>3.63</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A135" s="5">
         <v>37755</v>
       </c>
-    </row>
-    <row r="136" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B135">
+        <v>3.02</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A136" s="5">
         <v>37756</v>
       </c>
-    </row>
-    <row r="137" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B136">
+        <v>2.1800000000000002</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A137" s="5">
         <v>37757</v>
       </c>
-    </row>
-    <row r="138" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B137">
+        <v>1.72</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A138" s="5">
         <v>37758</v>
       </c>
-    </row>
-    <row r="139" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B138">
+        <v>1.56</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A139" s="5">
         <v>37759</v>
       </c>
-    </row>
-    <row r="140" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B139">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A140" s="5">
         <v>37760</v>
       </c>
-    </row>
-    <row r="141" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B140">
+        <v>1.89</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A141" s="5">
         <v>37761</v>
       </c>
-    </row>
-    <row r="142" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B141">
+        <v>3.55</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A142" s="5">
         <v>37762</v>
       </c>
-    </row>
-    <row r="143" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B142">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A143" s="5">
         <v>37763</v>
       </c>
-    </row>
-    <row r="144" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B143">
+        <v>1.72</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A144" s="5">
         <v>37764</v>
       </c>
-    </row>
-    <row r="145" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B144">
+        <v>1.45</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A145" s="5">
         <v>37765</v>
       </c>
-    </row>
-    <row r="146" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B145">
+        <v>1.66</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A146" s="5">
         <v>37766</v>
       </c>
-    </row>
-    <row r="147" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B146">
+        <v>2.19</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A147" s="5">
         <v>37767</v>
       </c>
-    </row>
-    <row r="148" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B147">
+        <v>2.52</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A148" s="5">
         <v>37768</v>
       </c>
-    </row>
-    <row r="149" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B148">
+        <v>2.87</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A149" s="5">
         <v>37769</v>
       </c>
-    </row>
-    <row r="150" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B149">
+        <v>4.21</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A150" s="5">
         <v>37770</v>
       </c>
-    </row>
-    <row r="151" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B150">
+        <v>5.01</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A151" s="5">
         <v>37771</v>
       </c>
-    </row>
-    <row r="152" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B151">
+        <v>4.76</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A152" s="5">
         <v>37772</v>
       </c>
-    </row>
-    <row r="153" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B152">
+        <v>5.98</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A153" s="5">
         <v>37773</v>
       </c>
     </row>
-    <row r="154" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A154" s="5">
         <v>37774</v>
       </c>
     </row>
-    <row r="155" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A155" s="5">
         <v>37775</v>
       </c>
     </row>
-    <row r="156" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A156" s="5">
         <v>37776</v>
       </c>
     </row>
-    <row r="157" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A157" s="5">
         <v>37777</v>
       </c>
     </row>
-    <row r="158" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A158" s="5">
         <v>37778</v>
       </c>
     </row>
-    <row r="159" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A159" s="5">
         <v>37779</v>
       </c>
     </row>
-    <row r="160" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A160" s="5">
         <v>37780</v>
       </c>

</xml_diff>

<commit_message>
workaround for working directory issue
</commit_message>
<xml_diff>
--- a/data/daily_runoff/12256_Rosegbach_example_river_runoff.xlsx
+++ b/data/daily_runoff/12256_Rosegbach_example_river_runoff.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10114"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB30742-1B04-174B-BD00-51B8B933B54D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAFAD47E-5088-AA4C-A739-4BFB51273DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20240" yWindow="800" windowWidth="10000" windowHeight="17180" tabRatio="841" firstSheet="20" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31292,8 +31292,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:B366"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
-      <selection activeCell="B153" sqref="B153"/>
+    <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
+      <selection activeCell="B214" sqref="B214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -32522,367 +32522,489 @@
       <c r="A153" s="1">
         <v>44713</v>
       </c>
-      <c r="B153" s="12"/>
+      <c r="B153" s="12">
+        <v>2.4</v>
+      </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A154" s="1">
         <v>44714</v>
       </c>
-      <c r="B154" s="12"/>
+      <c r="B154" s="12">
+        <v>3.08</v>
+      </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A155" s="1">
         <v>44715</v>
       </c>
-      <c r="B155" s="12"/>
+      <c r="B155" s="12">
+        <v>4.72</v>
+      </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A156" s="1">
         <v>44716</v>
       </c>
-      <c r="B156" s="12"/>
+      <c r="B156" s="12">
+        <v>6.34</v>
+      </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A157" s="1">
         <v>44717</v>
       </c>
-      <c r="B157" s="12"/>
+      <c r="B157" s="12">
+        <v>6.93</v>
+      </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A158" s="1">
         <v>44718</v>
       </c>
-      <c r="B158" s="12"/>
+      <c r="B158" s="12">
+        <v>6.41</v>
+      </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159" s="1">
         <v>44719</v>
       </c>
-      <c r="B159" s="12"/>
+      <c r="B159" s="12">
+        <v>6.38</v>
+      </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160" s="1">
         <v>44720</v>
       </c>
-      <c r="B160" s="12"/>
+      <c r="B160" s="12">
+        <v>4.97</v>
+      </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A161" s="1">
         <v>44721</v>
       </c>
-      <c r="B161" s="14"/>
+      <c r="B161" s="13">
+        <v>4.1100000000000003</v>
+      </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A162" s="1">
         <v>44722</v>
       </c>
-      <c r="B162" s="12"/>
+      <c r="B162" s="12">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A163" s="1">
         <v>44723</v>
       </c>
-      <c r="B163" s="12"/>
+      <c r="B163" s="12">
+        <v>3.76</v>
+      </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164" s="1">
         <v>44724</v>
       </c>
-      <c r="B164" s="12"/>
+      <c r="B164" s="12">
+        <v>4.18</v>
+      </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165" s="1">
         <v>44725</v>
       </c>
-      <c r="B165" s="12"/>
+      <c r="B165" s="12">
+        <v>5.0199999999999996</v>
+      </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166" s="1">
         <v>44726</v>
       </c>
-      <c r="B166" s="12"/>
+      <c r="B166" s="12">
+        <v>4.99</v>
+      </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
         <v>44727</v>
       </c>
-      <c r="B167" s="12"/>
+      <c r="B167" s="12">
+        <v>5.33</v>
+      </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A168" s="1">
         <v>44728</v>
       </c>
-      <c r="B168" s="12"/>
+      <c r="B168" s="12">
+        <v>5.88</v>
+      </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A169" s="1">
         <v>44729</v>
       </c>
-      <c r="B169" s="12"/>
+      <c r="B169" s="12">
+        <v>6.09</v>
+      </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A170" s="1">
         <v>44730</v>
       </c>
-      <c r="B170" s="12"/>
+      <c r="B170" s="12">
+        <v>6.22</v>
+      </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A171" s="1">
         <v>44731</v>
       </c>
-      <c r="B171" s="12"/>
+      <c r="B171" s="12">
+        <v>7.43</v>
+      </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A172" s="1">
         <v>44732</v>
       </c>
-      <c r="B172" s="12"/>
+      <c r="B172" s="12">
+        <v>7.89</v>
+      </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A173" s="1">
         <v>44733</v>
       </c>
-      <c r="B173" s="12"/>
+      <c r="B173" s="12">
+        <v>8.33</v>
+      </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A174" s="1">
         <v>44734</v>
       </c>
-      <c r="B174" s="12"/>
+      <c r="B174" s="12">
+        <v>10.4</v>
+      </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A175" s="1">
         <v>44735</v>
       </c>
-      <c r="B175" s="12"/>
+      <c r="B175" s="12">
+        <v>9.51</v>
+      </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A176" s="1">
         <v>44736</v>
       </c>
-      <c r="B176" s="12"/>
+      <c r="B176" s="12">
+        <v>8.6999999999999993</v>
+      </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A177" s="1">
         <v>44737</v>
       </c>
-      <c r="B177" s="12"/>
+      <c r="B177" s="12">
+        <v>7.53</v>
+      </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A178" s="1">
         <v>44738</v>
       </c>
-      <c r="B178" s="12"/>
+      <c r="B178" s="12">
+        <v>7.04</v>
+      </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A179" s="1">
         <v>44739</v>
       </c>
-      <c r="B179" s="12"/>
+      <c r="B179" s="12">
+        <v>9.0500000000000007</v>
+      </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A180" s="1">
         <v>44740</v>
       </c>
-      <c r="B180" s="12"/>
+      <c r="B180" s="12">
+        <v>9.67</v>
+      </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A181" s="1">
         <v>44741</v>
       </c>
-      <c r="B181" s="12"/>
+      <c r="B181" s="12">
+        <v>10.3</v>
+      </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A182" s="1">
         <v>44742</v>
       </c>
-      <c r="B182" s="12"/>
+      <c r="B182" s="12">
+        <v>8.58</v>
+      </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A183" s="1">
         <v>44743</v>
       </c>
-      <c r="B183" s="12"/>
+      <c r="B183" s="12">
+        <v>8</v>
+      </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A184" s="1">
         <v>44744</v>
       </c>
-      <c r="B184" s="12"/>
+      <c r="B184" s="12">
+        <v>7.32</v>
+      </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A185" s="1">
         <v>44745</v>
       </c>
-      <c r="B185" s="12"/>
+      <c r="B185" s="12">
+        <v>7.95</v>
+      </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A186" s="1">
         <v>44746</v>
       </c>
-      <c r="B186" s="12"/>
+      <c r="B186" s="12">
+        <v>9.9</v>
+      </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A187" s="1">
         <v>44747</v>
       </c>
-      <c r="B187" s="12"/>
+      <c r="B187" s="12">
+        <v>7.82</v>
+      </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A188" s="1">
         <v>44748</v>
       </c>
-      <c r="B188" s="12"/>
+      <c r="B188" s="12">
+        <v>7.26</v>
+      </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A189" s="1">
         <v>44749</v>
       </c>
-      <c r="B189" s="12"/>
+      <c r="B189" s="12">
+        <v>6.53</v>
+      </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A190" s="1">
         <v>44750</v>
       </c>
-      <c r="B190" s="12"/>
+      <c r="B190" s="12">
+        <v>6.19</v>
+      </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A191" s="1">
         <v>44751</v>
       </c>
-      <c r="B191" s="12"/>
+      <c r="B191" s="12">
+        <v>6.12</v>
+      </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A192" s="1">
         <v>44752</v>
       </c>
-      <c r="B192" s="12"/>
+      <c r="B192" s="12">
+        <v>5.9</v>
+      </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A193" s="1">
         <v>44753</v>
       </c>
-      <c r="B193" s="12"/>
+      <c r="B193" s="12">
+        <v>6.27</v>
+      </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A194" s="1">
         <v>44754</v>
       </c>
-      <c r="B194" s="12"/>
+      <c r="B194" s="12">
+        <v>6.81</v>
+      </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A195" s="1">
         <v>44755</v>
       </c>
-      <c r="B195" s="12"/>
+      <c r="B195" s="12">
+        <v>7.59</v>
+      </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A196" s="1">
         <v>44756</v>
       </c>
-      <c r="B196" s="12"/>
+      <c r="B196" s="12">
+        <v>8.1199999999999992</v>
+      </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A197" s="1">
         <v>44757</v>
       </c>
-      <c r="B197" s="12"/>
+      <c r="B197" s="12">
+        <v>8.56</v>
+      </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A198" s="1">
         <v>44758</v>
       </c>
-      <c r="B198" s="12"/>
+      <c r="B198" s="12">
+        <v>8.42</v>
+      </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A199" s="1">
         <v>44759</v>
       </c>
-      <c r="B199" s="12"/>
+      <c r="B199" s="12">
+        <v>8.06</v>
+      </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A200" s="1">
         <v>44760</v>
       </c>
-      <c r="B200" s="12"/>
+      <c r="B200" s="12">
+        <v>10.6</v>
+      </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A201" s="1">
         <v>44761</v>
       </c>
-      <c r="B201" s="14"/>
+      <c r="B201" s="14">
+        <v>11.1</v>
+      </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A202" s="1">
         <v>44762</v>
       </c>
-      <c r="B202" s="12"/>
+      <c r="B202" s="12">
+        <v>10.199999999999999</v>
+      </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A203" s="1">
         <v>44763</v>
       </c>
-      <c r="B203" s="12"/>
+      <c r="B203" s="12">
+        <v>12.6</v>
+      </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A204" s="1">
         <v>44764</v>
       </c>
-      <c r="B204" s="12"/>
+      <c r="B204" s="12">
+        <v>10.199999999999999</v>
+      </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A205" s="1">
         <v>44765</v>
       </c>
-      <c r="B205" s="12"/>
+      <c r="B205" s="12">
+        <v>12.2</v>
+      </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A206" s="1">
         <v>44766</v>
       </c>
-      <c r="B206" s="12"/>
+      <c r="B206" s="12">
+        <v>10.8</v>
+      </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A207" s="1">
         <v>44767</v>
       </c>
-      <c r="B207" s="12"/>
+      <c r="B207" s="12">
+        <v>8.2100000000000009</v>
+      </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A208" s="1">
         <v>44768</v>
       </c>
-      <c r="B208" s="12"/>
+      <c r="B208" s="12">
+        <v>8.34</v>
+      </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A209" s="1">
         <v>44769</v>
       </c>
-      <c r="B209" s="12"/>
+      <c r="B209" s="12">
+        <v>8.7100000000000009</v>
+      </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A210" s="1">
         <v>44770</v>
       </c>
-      <c r="B210" s="12"/>
+      <c r="B210" s="12">
+        <v>6.81</v>
+      </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A211" s="1">
         <v>44771</v>
       </c>
-      <c r="B211" s="12"/>
+      <c r="B211" s="12">
+        <v>5.68</v>
+      </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A212" s="1">
         <v>44772</v>
       </c>
-      <c r="B212" s="12"/>
+      <c r="B212" s="12">
+        <v>5.8</v>
+      </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A213" s="1">
         <v>44773</v>
       </c>
-      <c r="B213" s="12"/>
+      <c r="B213" s="12">
+        <v>5.9</v>
+      </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A214" s="1">

</xml_diff>

<commit_message>
still debugging the configuration tool internal paths
</commit_message>
<xml_diff>
--- a/data/daily_runoff/12256_Rosegbach_example_river_runoff.xlsx
+++ b/data/daily_runoff/12256_Rosegbach_example_river_runoff.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10114"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAFAD47E-5088-AA4C-A739-4BFB51273DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{755C1203-6CCC-E945-861D-9729ACA1FAD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20240" yWindow="800" windowWidth="10000" windowHeight="17180" tabRatio="841" firstSheet="20" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20620" yWindow="760" windowWidth="10000" windowHeight="17180" tabRatio="841" firstSheet="20" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2000" sheetId="9" r:id="rId1"/>
@@ -31292,8 +31292,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:B366"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
-      <selection activeCell="B214" sqref="B214"/>
+    <sheetView tabSelected="1" topLeftCell="A272" workbookViewId="0">
+      <selection activeCell="B275" sqref="B275"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -33010,367 +33010,489 @@
       <c r="A214" s="1">
         <v>44774</v>
       </c>
-      <c r="B214" s="12"/>
+      <c r="B214" s="12">
+        <v>6.44</v>
+      </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A215" s="1">
         <v>44775</v>
       </c>
-      <c r="B215" s="12"/>
+      <c r="B215" s="12">
+        <v>7.43</v>
+      </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A216" s="1">
         <v>44776</v>
       </c>
-      <c r="B216" s="12"/>
+      <c r="B216" s="12">
+        <v>7.24</v>
+      </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A217" s="1">
         <v>44777</v>
       </c>
-      <c r="B217" s="12"/>
+      <c r="B217" s="12">
+        <v>8.44</v>
+      </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A218" s="1">
         <v>44778</v>
       </c>
-      <c r="B218" s="12"/>
+      <c r="B218" s="12">
+        <v>9.16</v>
+      </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A219" s="1">
         <v>44779</v>
       </c>
-      <c r="B219" s="12"/>
+      <c r="B219" s="12">
+        <v>7.68</v>
+      </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A220" s="1">
         <v>44780</v>
       </c>
-      <c r="B220" s="12"/>
+      <c r="B220" s="12">
+        <v>7.1</v>
+      </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A221" s="1">
         <v>44781</v>
       </c>
-      <c r="B221" s="12"/>
+      <c r="B221" s="12">
+        <v>6.54</v>
+      </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A222" s="1">
         <v>44782</v>
       </c>
-      <c r="B222" s="12"/>
+      <c r="B222" s="12">
+        <v>6.57</v>
+      </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A223" s="1">
         <v>44783</v>
       </c>
-      <c r="B223" s="12"/>
+      <c r="B223" s="12">
+        <v>6.29</v>
+      </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A224" s="1">
         <v>44784</v>
       </c>
-      <c r="B224" s="12"/>
+      <c r="B224" s="12">
+        <v>6.36</v>
+      </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A225" s="1">
         <v>44785</v>
       </c>
-      <c r="B225" s="12"/>
+      <c r="B225" s="12">
+        <v>6.05</v>
+      </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A226" s="1">
         <v>44786</v>
       </c>
-      <c r="B226" s="12"/>
+      <c r="B226" s="12">
+        <v>5.5</v>
+      </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A227" s="1">
         <v>44787</v>
       </c>
-      <c r="B227" s="12"/>
+      <c r="B227" s="12">
+        <v>5.2</v>
+      </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A228" s="1">
         <v>44788</v>
       </c>
-      <c r="B228" s="12"/>
+      <c r="B228" s="12">
+        <v>5.34</v>
+      </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A229" s="1">
         <v>44789</v>
       </c>
-      <c r="B229" s="12"/>
+      <c r="B229" s="12">
+        <v>5.23</v>
+      </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A230" s="1">
         <v>44790</v>
       </c>
-      <c r="B230" s="12"/>
+      <c r="B230" s="12">
+        <v>5.69</v>
+      </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A231" s="1">
         <v>44791</v>
       </c>
-      <c r="B231" s="12"/>
+      <c r="B231" s="12">
+        <v>7.94</v>
+      </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A232" s="1">
         <v>44792</v>
       </c>
-      <c r="B232" s="12"/>
+      <c r="B232" s="12">
+        <v>5.91</v>
+      </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A233" s="1">
         <v>44793</v>
       </c>
-      <c r="B233" s="12"/>
+      <c r="B233" s="12">
+        <v>5.25</v>
+      </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A234" s="1">
         <v>44794</v>
       </c>
-      <c r="B234" s="12"/>
+      <c r="B234" s="12">
+        <v>5.09</v>
+      </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A235" s="1">
         <v>44795</v>
       </c>
-      <c r="B235" s="12"/>
+      <c r="B235" s="12">
+        <v>4.74</v>
+      </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A236" s="1">
         <v>44796</v>
       </c>
-      <c r="B236" s="12"/>
+      <c r="B236" s="12">
+        <v>4.7</v>
+      </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A237" s="1">
         <v>44797</v>
       </c>
-      <c r="B237" s="12"/>
+      <c r="B237" s="12">
+        <v>4.71</v>
+      </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A238" s="1">
         <v>44798</v>
       </c>
-      <c r="B238" s="12"/>
+      <c r="B238" s="12">
+        <v>4.8899999999999997</v>
+      </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A239" s="1">
         <v>44799</v>
       </c>
-      <c r="B239" s="12"/>
+      <c r="B239" s="12">
+        <v>5.14</v>
+      </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A240" s="1">
         <v>44800</v>
       </c>
-      <c r="B240" s="12"/>
+      <c r="B240" s="12">
+        <v>5.5</v>
+      </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A241" s="1">
         <v>44801</v>
       </c>
-      <c r="B241" s="15"/>
+      <c r="B241" s="15">
+        <v>5.29</v>
+      </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A242" s="1">
         <v>44802</v>
       </c>
-      <c r="B242" s="12"/>
+      <c r="B242" s="12">
+        <v>5.41</v>
+      </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A243" s="1">
         <v>44803</v>
       </c>
-      <c r="B243" s="12"/>
+      <c r="B243" s="12">
+        <v>5.24</v>
+      </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A244" s="1">
         <v>44804</v>
       </c>
-      <c r="B244" s="12"/>
+      <c r="B244" s="12">
+        <v>4.84</v>
+      </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A245" s="1">
         <v>44805</v>
       </c>
-      <c r="B245" s="12"/>
+      <c r="B245" s="12">
+        <v>4.17</v>
+      </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A246" s="1">
         <v>44806</v>
       </c>
-      <c r="B246" s="12"/>
+      <c r="B246" s="12">
+        <v>3.82</v>
+      </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A247" s="1">
         <v>44807</v>
       </c>
-      <c r="B247" s="12"/>
+      <c r="B247" s="12">
+        <v>4.46</v>
+      </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A248" s="1">
         <v>44808</v>
       </c>
-      <c r="B248" s="12"/>
+      <c r="B248" s="12">
+        <v>3.68</v>
+      </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A249" s="1">
         <v>44809</v>
       </c>
-      <c r="B249" s="12"/>
+      <c r="B249" s="12">
+        <v>3.62</v>
+      </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A250" s="1">
         <v>44810</v>
       </c>
-      <c r="B250" s="12"/>
+      <c r="B250" s="12">
+        <v>4.0199999999999996</v>
+      </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A251" s="1">
         <v>44811</v>
       </c>
-      <c r="B251" s="12"/>
+      <c r="B251" s="12">
+        <v>4.9400000000000004</v>
+      </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A252" s="1">
         <v>44812</v>
       </c>
-      <c r="B252" s="16"/>
+      <c r="B252" s="16">
+        <v>8.82</v>
+      </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A253" s="1">
         <v>44813</v>
       </c>
-      <c r="B253" s="16"/>
+      <c r="B253" s="16">
+        <v>5.68</v>
+      </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A254" s="1">
         <v>44814</v>
       </c>
-      <c r="B254" s="16"/>
+      <c r="B254" s="16">
+        <v>3.96</v>
+      </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A255" s="1">
         <v>44815</v>
       </c>
-      <c r="B255" s="16"/>
+      <c r="B255" s="16">
+        <v>2.99</v>
+      </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A256" s="1">
         <v>44816</v>
       </c>
-      <c r="B256" s="16"/>
+      <c r="B256" s="16">
+        <v>2.4700000000000002</v>
+      </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A257" s="1">
         <v>44817</v>
       </c>
-      <c r="B257" s="16"/>
+      <c r="B257" s="16">
+        <v>2.57</v>
+      </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A258" s="1">
         <v>44818</v>
       </c>
-      <c r="B258" s="16"/>
+      <c r="B258" s="16">
+        <v>4.18</v>
+      </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A259" s="1">
         <v>44819</v>
       </c>
-      <c r="B259" s="16"/>
+      <c r="B259" s="16">
+        <v>4.71</v>
+      </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A260" s="1">
         <v>44820</v>
       </c>
-      <c r="B260" s="16"/>
+      <c r="B260" s="16">
+        <v>3.66</v>
+      </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A261" s="1">
         <v>44821</v>
       </c>
-      <c r="B261" s="16"/>
+      <c r="B261" s="16">
+        <v>2.42</v>
+      </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A262" s="1">
         <v>44822</v>
       </c>
-      <c r="B262" s="16"/>
+      <c r="B262" s="16">
+        <v>1.68</v>
+      </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A263" s="1">
         <v>44823</v>
       </c>
-      <c r="B263" s="16"/>
+      <c r="B263" s="16">
+        <v>1.45</v>
+      </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A264" s="1">
         <v>44824</v>
       </c>
-      <c r="B264" s="16"/>
+      <c r="B264" s="16">
+        <v>1.3</v>
+      </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A265" s="1">
         <v>44825</v>
       </c>
-      <c r="B265" s="16"/>
+      <c r="B265" s="16">
+        <v>1.22</v>
+      </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A266" s="1">
         <v>44826</v>
       </c>
-      <c r="B266" s="16"/>
+      <c r="B266" s="16">
+        <v>1.18</v>
+      </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A267" s="1">
         <v>44827</v>
       </c>
-      <c r="B267" s="16"/>
+      <c r="B267" s="16">
+        <v>1.1399999999999999</v>
+      </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A268" s="1">
         <v>44828</v>
       </c>
-      <c r="B268" s="16"/>
+      <c r="B268" s="16">
+        <v>1.06</v>
+      </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A269" s="1">
         <v>44829</v>
       </c>
-      <c r="B269" s="16"/>
+      <c r="B269" s="16">
+        <v>0.97</v>
+      </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A270" s="1">
         <v>44830</v>
       </c>
-      <c r="B270" s="16"/>
+      <c r="B270" s="16">
+        <v>0.93</v>
+      </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A271" s="1">
         <v>44831</v>
       </c>
-      <c r="B271" s="16"/>
+      <c r="B271" s="16">
+        <v>0.83</v>
+      </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A272" s="1">
         <v>44832</v>
       </c>
-      <c r="B272" s="16"/>
+      <c r="B272" s="16">
+        <v>0.76</v>
+      </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A273" s="1">
         <v>44833</v>
       </c>
-      <c r="B273" s="16"/>
+      <c r="B273" s="16">
+        <v>0.73</v>
+      </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A274" s="1">
         <v>44834</v>
       </c>
-      <c r="B274" s="16"/>
+      <c r="B274" s="16">
+        <v>0.74</v>
+      </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A275" s="1">

</xml_diff>